<commit_message>
made small changes to excell sheet
</commit_message>
<xml_diff>
--- a/analysis/algo_compare.xlsx
+++ b/analysis/algo_compare.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\GitRepos\ML-final_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\GitRepos\ML-final_proj\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -67,7 +67,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,15 +100,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -245,7 +255,7 @@
             <c:numRef>
               <c:f>Compare!$B$2:$B$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.28447</c:v>
@@ -316,7 +326,7 @@
             <c:numRef>
               <c:f>Compare!$C$2:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.24202000000000001</c:v>
@@ -479,7 +489,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2789,7 +2799,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,10 +2827,10 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.28447</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.24202000000000001</v>
       </c>
       <c r="D2">
@@ -2831,10 +2841,10 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0.21426000000000001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.21185000000000001</v>
       </c>
       <c r="D3">
@@ -2845,10 +2855,10 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0.17938999999999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.17829999999999999</v>
       </c>
       <c r="D4">
@@ -2859,10 +2869,10 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>0.22931000000000001</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.22802</v>
       </c>
       <c r="D5">
@@ -2871,6 +2881,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>